<commit_message>
添加netswift板卡适配 openEuler 22.03 LTS SP3版本测试结果
</commit_message>
<xml_diff>
--- a/data/compatibility/openEuler22.03-LTS-SP3上两类平台板卡兼容清单.xlsx
+++ b/data/compatibility/openEuler22.03-LTS-SP3上两类平台板卡兼容清单.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20745" windowHeight="9675" tabRatio="500"/>
+    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openEuler22.03-LTS-SP3两类平台板卡兼容性" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="95">
   <si>
     <t>vendorID</t>
   </si>
@@ -191,6 +191,126 @@
   </si>
   <si>
     <t>QLE2772</t>
+  </si>
+  <si>
+    <t>8088</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>txgbe</t>
+  </si>
+  <si>
+    <t>1.3.2oe</t>
+  </si>
+  <si>
+    <t>NIC</t>
+  </si>
+  <si>
+    <t>91049901f1c0c1f717b646505ffb9c066fda004932e6031ab5dcc7ed336f9358</t>
+  </si>
+  <si>
+    <t>95K</t>
+  </si>
+  <si>
+    <t>Netswift</t>
+  </si>
+  <si>
+    <t>RP1000P2SFP</t>
+  </si>
+  <si>
+    <t>SP1000A</t>
+  </si>
+  <si>
+    <t>inbox</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>RP2000P2SFP</t>
+  </si>
+  <si>
+    <t>WX1820AL</t>
+  </si>
+  <si>
+    <t>0105</t>
+  </si>
+  <si>
+    <t>0202</t>
+  </si>
+  <si>
+    <t>ngbe</t>
+  </si>
+  <si>
+    <t>1.2.2oe</t>
+  </si>
+  <si>
+    <t>9b3a6c73035fcdd4596c8236c827369a01778ab3ce807a2451c7c98fc4cbe9f8</t>
+  </si>
+  <si>
+    <t>87K</t>
+  </si>
+  <si>
+    <t>SF200HT</t>
+  </si>
+  <si>
+    <t>WX1860AL2</t>
+  </si>
+  <si>
+    <t>0101</t>
+  </si>
+  <si>
+    <t>0201</t>
+  </si>
+  <si>
+    <t>SF200T</t>
+  </si>
+  <si>
+    <t>WX1860A2</t>
+  </si>
+  <si>
+    <t>0107</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>SF400HT</t>
+  </si>
+  <si>
+    <t>WX1860AL4</t>
+  </si>
+  <si>
+    <t>0401</t>
+  </si>
+  <si>
+    <t>SF400T</t>
+  </si>
+  <si>
+    <t>WX1860A4</t>
+  </si>
+  <si>
+    <t>39d480b1ca092fb4bc01732d077525a595b8b2ed3b63fb5d9c6bd21dab290d1b</t>
+  </si>
+  <si>
+    <t>107K</t>
+  </si>
+  <si>
+    <t>b0c9650549a49fc6bc1b37a6a1f06a528f41d13174b2777883a0da03ab435fc4</t>
+  </si>
+  <si>
+    <t>97K</t>
+  </si>
+  <si>
+    <t>0103</t>
   </si>
   <si>
     <t>板卡</t>
@@ -1328,10 +1448,10 @@
   <sheetPr/>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2283,226 +2403,616 @@
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="15"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="17"/>
+      <c r="A19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="P19" s="24"/>
-      <c r="Q19" s="17"/>
+      <c r="Q19" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="15"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="17"/>
+      <c r="A20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="P20" s="24"/>
-      <c r="Q20" s="17"/>
+      <c r="Q20" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="15"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="17"/>
+      <c r="A21" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O21" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="P21" s="24"/>
-      <c r="Q21" s="17"/>
+      <c r="Q21" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="17"/>
+      <c r="A22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L22" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" s="17" t="s">
+        <v>80</v>
+      </c>
       <c r="P22" s="24"/>
-      <c r="Q22" s="17"/>
+      <c r="Q22" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="17"/>
+      <c r="A23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="O23" s="17" t="s">
+        <v>84</v>
+      </c>
       <c r="P23" s="24"/>
-      <c r="Q23" s="17"/>
+      <c r="Q23" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="15"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="17"/>
+      <c r="A24" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="O24" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="P24" s="24"/>
-      <c r="Q24" s="17"/>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="19"/>
-    </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="19"/>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="18"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="18"/>
-      <c r="P27" s="19"/>
-    </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18"/>
-      <c r="O28" s="18"/>
-      <c r="P28" s="19"/>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
-      <c r="P29" s="19"/>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="19"/>
+      <c r="Q24" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="O25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="L26" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="O26" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="L27" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O27" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="L28" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="L29" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="O29" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="L30" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="O30" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="17" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="18"/>
@@ -2737,10 +3247,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" ht="27" customHeight="1"/>

</xml_diff>